<commit_message>
updated api docs with alpha tests
</commit_message>
<xml_diff>
--- a/Api Documentation Samples.xlsx
+++ b/Api Documentation Samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\naylinnmaung\phone-pos-nay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212C59AF-EC08-48C2-AE64-6D4A8E807267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A637D261-25C1-4D44-8328-23AB2558B3CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D655E72-7771-439B-A6BC-B8D33FCB89D2}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="89">
   <si>
     <t>Id</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>//later and not used</t>
+  </si>
+  <si>
+    <t>/dashboard</t>
+  </si>
+  <si>
+    <t>I have no idea</t>
+  </si>
+  <si>
+    <t>It is in beta. Just try and feedback.</t>
   </si>
 </sst>
 </file>
@@ -452,6 +461,13 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -461,17 +477,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FC7D299-354C-4E80-92A4-1CCB40503251}">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A2:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -820,14 +829,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -883,79 +892,79 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7">
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    <row r="8" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
+    <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -997,7 +1006,7 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E13" t="s">
@@ -1028,7 +1037,7 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="1" t="s">
         <v>76</v>
       </c>
       <c r="E15" t="s">
@@ -1073,7 +1082,7 @@
       <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
       <c r="E18" t="s">
@@ -1104,7 +1113,7 @@
       <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E20" t="s">
@@ -1149,7 +1158,7 @@
       <c r="C23" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="1" t="s">
         <v>79</v>
       </c>
       <c r="E23" t="s">
@@ -1180,7 +1189,7 @@
       <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E25" t="s">
@@ -1225,7 +1234,7 @@
       <c r="C28" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E28" t="s">
@@ -1256,7 +1265,7 @@
       <c r="C30" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E30" t="s">
@@ -1291,7 +1300,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1301,14 +1310,14 @@
       <c r="C33" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="1" t="s">
         <v>83</v>
       </c>
       <c r="E33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1332,14 +1341,14 @@
       <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="1" t="s">
         <v>84</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1373,7 +1382,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1388,6 +1397,26 @@
       </c>
       <c r="E38" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1413,246 +1442,246 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1674,246 +1703,246 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="5" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1935,246 +1964,246 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="5" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="3:14" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2196,246 +2225,246 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2457,246 +2486,246 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
     </row>
     <row r="16" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>